<commit_message>
final draft for Bahir Dar part 1
</commit_message>
<xml_diff>
--- a/Handouts/Spreadsheets/2D Water Flow.xlsx
+++ b/Handouts/Spreadsheets/2D Water Flow.xlsx
@@ -91,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -179,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +464,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,47 +1588,47 @@
       </c>
       <c r="C33" s="10">
         <f ca="1">(2*C34+D33+B33)/4</f>
-        <v>1.5848192634499358</v>
+        <v>1.5848192634570424</v>
       </c>
       <c r="D33" s="10">
         <f t="shared" ref="D33:M33" ca="1" si="31">(2*D34+E33+C33)/4</f>
-        <v>1.5396112067180023</v>
+        <v>1.5396112067312746</v>
       </c>
       <c r="E33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.4884692893255003</v>
+        <v>1.4884692893436537</v>
       </c>
       <c r="F33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.4279489210321392</v>
+        <v>1.4279489210536522</v>
       </c>
       <c r="G33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.3540150829694564</v>
+        <v>1.3540150829926851</v>
       </c>
       <c r="H33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.2618320024349277</v>
+        <v>1.2618320024582219</v>
       </c>
       <c r="I33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.1455882173896654</v>
+        <v>1.1455882174114751</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>0.99847639144967526</v>
+        <v>0.99847639146864275</v>
       </c>
       <c r="K33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>0.81314217628325181</v>
+        <v>0.81314217629828511</v>
       </c>
       <c r="L33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>0.583333884354309</v>
+        <v>0.58333388436463185</v>
       </c>
       <c r="M33" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>0.30813096760613545</v>
+        <v>0.30813096761132197</v>
       </c>
       <c r="N33" s="10">
         <v>0</v>
@@ -1643,47 +1643,47 @@
       </c>
       <c r="C34" s="10">
         <f t="shared" ref="C34" ca="1" si="32">(C33+C35+D34+B34)/4</f>
-        <v>1.5862557108858011</v>
+        <v>1.5862557108924336</v>
       </c>
       <c r="D34" s="10">
         <f t="shared" ref="D34" ca="1" si="33">(D33+D35+E34+C34)/4</f>
-        <v>1.5425781370601774</v>
+        <v>1.5425781370725646</v>
       </c>
       <c r="E34" s="10">
         <f t="shared" ref="E34" ca="1" si="34">(E33+E35+F34+D34)/4</f>
-        <v>1.4931585147912747</v>
+        <v>1.4931585148082183</v>
       </c>
       <c r="F34" s="10">
         <f t="shared" ref="F34" ca="1" si="35">(F33+F35+G34+E34)/4</f>
-        <v>1.434655655934358</v>
+        <v>1.4346556559544379</v>
       </c>
       <c r="G34" s="10">
         <f t="shared" ref="G34" ca="1" si="36">(G33+G35+H34+F34)/4</f>
-        <v>1.3631397042238433</v>
+        <v>1.3631397042455256</v>
       </c>
       <c r="H34" s="10">
         <f t="shared" ref="H34" ca="1" si="37">(H33+H35+I34+G34)/4</f>
-        <v>1.273862354708382</v>
+        <v>1.2738623547301282</v>
       </c>
       <c r="I34" s="10">
         <f t="shared" ref="I34" ca="1" si="38">(I33+I35+J34+H34)/4</f>
-        <v>1.1610222378535648</v>
+        <v>1.1610222378739294</v>
       </c>
       <c r="J34" s="10">
         <f t="shared" ref="J34" ca="1" si="39">(J33+J35+K34+I34)/4</f>
-        <v>1.0175875860768713</v>
+        <v>1.0175875860945895</v>
       </c>
       <c r="K34" s="10">
         <f t="shared" ref="K34" ca="1" si="40">(K33+K35+L34+J34)/4</f>
-        <v>0.83537921467515663</v>
+        <v>0.83537921468921073</v>
       </c>
       <c r="L34" s="10">
         <f t="shared" ref="L34" ca="1" si="41">(L33+L35+M34+K34)/4</f>
-        <v>0.60603119677071449</v>
+        <v>0.60603119678037842</v>
       </c>
       <c r="M34" s="10">
         <f t="shared" ref="M34" ca="1" si="42">(M33+M35+N34+L34)/4</f>
-        <v>0.3245949930378117</v>
+        <v>0.32459499304267725</v>
       </c>
       <c r="N34" s="10">
         <v>0</v>
@@ -1698,47 +1698,47 @@
       </c>
       <c r="C35" s="10">
         <f t="shared" ref="C35:C38" ca="1" si="43">(C34+C36+D35+B35)/4</f>
-        <v>1.5904710177182964</v>
+        <v>1.5904710177240424</v>
       </c>
       <c r="D35" s="10">
         <f t="shared" ref="D35:D38" ca="1" si="44">(D34+D36+E35+C35)/4</f>
-        <v>1.5512871158609629</v>
+        <v>1.5512871158716952</v>
       </c>
       <c r="E35" s="10">
         <f t="shared" ref="E35:E38" ca="1" si="45">(E34+E36+F35+D35)/4</f>
-        <v>1.5069309768643193</v>
+        <v>1.5069309768789996</v>
       </c>
       <c r="F35" s="10">
         <f t="shared" ref="F35:F38" ca="1" si="46">(F34+F36+G35+E35)/4</f>
-        <v>1.4543754837118255</v>
+        <v>1.4543754837292246</v>
       </c>
       <c r="G35" s="10">
         <f t="shared" ref="G35:G38" ca="1" si="47">(G34+G36+H35+F35)/4</f>
-        <v>1.3900257233056332</v>
+        <v>1.3900257233244242</v>
       </c>
       <c r="H35" s="10">
         <f t="shared" ref="H35:H38" ca="1" si="48">(H34+H36+I35+G35)/4</f>
-        <v>1.3094554743429181</v>
+        <v>1.3094554743617706</v>
       </c>
       <c r="I35" s="10">
         <f t="shared" ref="I35:I38" ca="1" si="49">(I34+I36+J35+H35)/4</f>
-        <v>1.2070507932589432</v>
+        <v>1.2070507932766097</v>
       </c>
       <c r="J35" s="10">
         <f t="shared" ref="J35:J38" ca="1" si="50">(J34+J36+K35+I35)/4</f>
-        <v>1.0754725003454009</v>
+        <v>1.0754725003607926</v>
       </c>
       <c r="K35" s="10">
         <f t="shared" ref="K35:K38" ca="1" si="51">(K34+K36+L35+J35)/4</f>
-        <v>0.90475589958192426</v>
+        <v>0.90475589959416647</v>
       </c>
       <c r="L35" s="10">
         <f t="shared" ref="L35:L38" ca="1" si="52">(L34+L36+M35+K35)/4</f>
-        <v>0.68081669502296516</v>
+        <v>0.68081669503142961</v>
       </c>
       <c r="M35" s="10">
         <f t="shared" ref="M35:M38" ca="1" si="53">(M34+M36+N35+L35)/4</f>
-        <v>0.38421780777678194</v>
+        <v>0.38421780778108716</v>
       </c>
       <c r="N35" s="10">
         <v>0</v>
@@ -1753,47 +1753,47 @@
       </c>
       <c r="C36" s="10">
         <f t="shared" ca="1" si="43"/>
-        <v>1.5971868188100378</v>
+        <v>1.5971868188145717</v>
       </c>
       <c r="D36" s="10">
         <f t="shared" ca="1" si="44"/>
-        <v>1.5651683318138825</v>
+        <v>1.5651683318223506</v>
       </c>
       <c r="E36" s="10">
         <f t="shared" ca="1" si="45"/>
-        <v>1.5289027931092702</v>
+        <v>1.5289027931208541</v>
       </c>
       <c r="F36" s="10">
         <f t="shared" ca="1" si="46"/>
-        <v>1.4858895787610082</v>
+        <v>1.4858895787747393</v>
       </c>
       <c r="G36" s="10">
         <f t="shared" ca="1" si="47"/>
-        <v>1.4331322309626069</v>
+        <v>1.4331322309774406</v>
       </c>
       <c r="H36" s="10">
         <f t="shared" ca="1" si="48"/>
-        <v>1.3668830261167495</v>
+        <v>1.3668830261316391</v>
       </c>
       <c r="I36" s="10">
         <f t="shared" ca="1" si="49"/>
-        <v>1.2822529605101536</v>
+        <v>1.2822529605241222</v>
       </c>
       <c r="J36" s="10">
         <f t="shared" ca="1" si="50"/>
-        <v>1.1724957224774055</v>
+        <v>1.1724957224896062</v>
       </c>
       <c r="K36" s="10">
         <f t="shared" ca="1" si="51"/>
-        <v>1.0273551882942713</v>
+        <v>1.0273551883040333</v>
       </c>
       <c r="L36" s="10">
         <f t="shared" ca="1" si="52"/>
-        <v>0.82826187596862122</v>
+        <v>0.82826187597547396</v>
       </c>
       <c r="M36" s="10">
         <f t="shared" ca="1" si="53"/>
-        <v>0.53145954304836318</v>
+        <v>0.5314595430519955</v>
       </c>
       <c r="N36" s="10">
         <v>0</v>
@@ -1808,51 +1808,51 @@
       </c>
       <c r="C37" s="10">
         <f t="shared" ca="1" si="43"/>
-        <v>1.6059535003895395</v>
+        <v>1.6059535003926377</v>
       </c>
       <c r="D37" s="10">
         <f t="shared" ca="1" si="44"/>
-        <v>1.583296599484882</v>
+        <v>1.5832965994906687</v>
       </c>
       <c r="E37" s="10">
         <f t="shared" ca="1" si="45"/>
-        <v>1.557622285009862</v>
+        <v>1.5576222850177781</v>
       </c>
       <c r="F37" s="10">
         <f t="shared" ca="1" si="46"/>
-        <v>1.5271478072737468</v>
+        <v>1.5271478072831317</v>
       </c>
       <c r="G37" s="10">
         <f t="shared" ca="1" si="47"/>
-        <v>1.489730595680903</v>
+        <v>1.4897305956910447</v>
       </c>
       <c r="H37" s="10">
         <f t="shared" ca="1" si="48"/>
-        <v>1.4426914386647005</v>
+        <v>1.4426914386748866</v>
       </c>
       <c r="I37" s="10">
         <f t="shared" ca="1" si="49"/>
-        <v>1.3825823001995761</v>
+        <v>1.3825823002091453</v>
       </c>
       <c r="J37" s="10">
         <f t="shared" ca="1" si="50"/>
-        <v>1.3049022407698514</v>
+        <v>1.3049022407782398</v>
       </c>
       <c r="K37" s="10">
         <f t="shared" ca="1" si="51"/>
-        <v>1.2039072551566874</v>
+        <v>1.2039072551634697</v>
       </c>
       <c r="L37" s="10">
         <f t="shared" ca="1" si="52"/>
-        <v>1.0734160775136352</v>
+        <v>1.0734160775185773</v>
       </c>
       <c r="M37" s="10">
         <f t="shared" ca="1" si="53"/>
-        <v>0.91335848844979339</v>
+        <v>0.91335848845294065</v>
       </c>
       <c r="N37" s="10">
         <f ca="1">(N36+N38+2*M37)/4</f>
-        <v>0.76653758819991846</v>
+        <v>0.7665375882018638</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -1864,51 +1864,51 @@
       </c>
       <c r="C38" s="10">
         <f t="shared" ca="1" si="43"/>
-        <v>1.6161761579424623</v>
+        <v>1.6161761579440119</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" ca="1" si="44"/>
-        <v>1.6044422807322332</v>
+        <v>1.6044422807351275</v>
       </c>
       <c r="E38" s="10">
         <f t="shared" ca="1" si="45"/>
-        <v>1.5911419401789417</v>
+        <v>1.5911419401829014</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" ca="1" si="46"/>
-        <v>1.5753487696514323</v>
+        <v>1.5753487696561275</v>
       </c>
       <c r="G38" s="10">
         <f t="shared" ca="1" si="47"/>
-        <v>1.5559509058310124</v>
+        <v>1.5559509058360872</v>
       </c>
       <c r="H38" s="10">
         <f t="shared" ca="1" si="48"/>
-        <v>1.5315698326696994</v>
+        <v>1.5315698326747993</v>
       </c>
       <c r="I38" s="10">
         <f t="shared" ca="1" si="49"/>
-        <v>1.5004825608609025</v>
+        <v>1.5004825608656991</v>
       </c>
       <c r="J38" s="10">
         <f t="shared" ca="1" si="50"/>
-        <v>1.4606236852518308</v>
+        <v>1.4606236852560484</v>
       </c>
       <c r="K38" s="10">
         <f t="shared" ca="1" si="51"/>
-        <v>1.4099555140536353</v>
+        <v>1.4099555140570756</v>
       </c>
       <c r="L38" s="10">
         <f t="shared" ca="1" si="52"/>
-        <v>1.3481366904826111</v>
+        <v>1.3481366904851897</v>
       </c>
       <c r="M38" s="10">
         <f t="shared" ca="1" si="53"/>
-        <v>1.2820207450393328</v>
+        <v>1.2820207450411361</v>
       </c>
       <c r="N38" s="10">
         <f ca="1">(N37+N39+2*M38)/4</f>
-        <v>1.239433375900856</v>
+        <v>1.239433375902244</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>